<commit_message>
feat(add sinkronisasi lokasi kabupaten)
</commit_message>
<xml_diff>
--- a/public/template/imb_perluasan_contoh.xlsx
+++ b/public/template/imb_perluasan_contoh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AC1EE2-210F-4312-AE35-808638250D4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47138A6A-50D5-48B3-BBE1-9C026021D503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3490" yWindow="1680" windowWidth="14400" windowHeight="7360" xr2:uid="{38E4490F-ED6A-D043-9D47-1EEDE93A9E56}"/>
+    <workbookView xWindow="1180" yWindow="1350" windowWidth="14400" windowHeight="8300" xr2:uid="{38E4490F-ED6A-D043-9D47-1EEDE93A9E56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -114,9 +114,6 @@
     <t>VILLA NUSA INDAH V</t>
   </si>
   <si>
-    <t>GUNUNG PUTRI</t>
-  </si>
-  <si>
     <t>Lt. I = 37 ; Lt. II = 39,50 ; b = 3,25 ; t = 8,5 ; p(k) = 25 ; p = 17</t>
   </si>
   <si>
@@ -132,13 +129,19 @@
     <t>Revisi Nama pertgl. 23/03/2009 ttd : kasi, kabid, kadis</t>
   </si>
   <si>
-    <t>CIANGSANA</t>
-  </si>
-  <si>
     <t>Kabupaten / Kota</t>
   </si>
   <si>
     <t>KOTA BOGOR</t>
+  </si>
+  <si>
+    <t>BOGOR SELATAN</t>
+  </si>
+  <si>
+    <t>CIPAKU</t>
+  </si>
+  <si>
+    <t>2009-11-10</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -251,9 +254,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -262,6 +262,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -582,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A055D-1491-2B4A-886A-82BCBACDCB92}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -630,8 +636,8 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
-        <v>34</v>
+      <c r="M1" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
@@ -668,14 +674,14 @@
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6">
-        <v>40097</v>
+      <c r="C2" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="11">
-        <v>40097</v>
+      <c r="E2" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="6"/>
@@ -685,42 +691,42 @@
       <c r="I2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>32</v>
+      <c r="V2" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fix bug in imb and rekap
</commit_message>
<xml_diff>
--- a/public/template/imb_perluasan_contoh.xlsx
+++ b/public/template/imb_perluasan_contoh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47138A6A-50D5-48B3-BBE1-9C026021D503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D14EBA1-02FA-49DC-A46B-62E8C6B81F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1350" windowWidth="14400" windowHeight="8300" xr2:uid="{38E4490F-ED6A-D043-9D47-1EEDE93A9E56}"/>
+    <workbookView xWindow="1640" yWindow="1230" windowWidth="14820" windowHeight="8300" xr2:uid="{38E4490F-ED6A-D043-9D47-1EEDE93A9E56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Jenis Kegiatan</t>
   </si>
   <si>
-    <t>Fungsi Kegiatan</t>
-  </si>
-  <si>
     <t>Lokasi / Perumahan</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>2009-11-10</t>
+  </si>
+  <si>
+    <t>Fungsi Bangunan</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -631,40 +631,40 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="93" x14ac:dyDescent="0.35">
@@ -672,61 +672,61 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="6"/>
       <c r="H2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>26</v>
-      </c>
       <c r="M2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="V2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>